<commit_message>
Some minor aesthetic changes to the sheet that is useful to humans and completely unreadable to R
</commit_message>
<xml_diff>
--- a/Data/-Asclepias-Indices.xlsx
+++ b/Data/-Asclepias-Indices.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick.lyon/Documents/_Publications/2021_Moranz_Asclepias/Moranz-AsclepiasCollab/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick.lyon/Documents/_Publications/2022_Moranz_Asclepias/Moranz-AsclepiasCollab/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A875A589-0007-2E45-BA1B-EDA01556A5BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBEAA242-41D8-A44A-A043-C89B007F1E18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="600" windowWidth="27360" windowHeight="16760" activeTab="3" xr2:uid="{11370D87-3625-934B-A86E-98D4B25C608F}"/>
   </bookViews>
@@ -7573,7 +7573,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I7" sqref="I7"/>
+      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Edited the tidy script to also process the relevant portion of the master GRG (Grand River Grasslands) butterfly surveys. That file is not included because it has not (yet) been published but you can see the path it follows to understand what was done.
</commit_message>
<xml_diff>
--- a/Data/-Asclepias-Indices.xlsx
+++ b/Data/-Asclepias-Indices.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick.lyon/Documents/_Publications/2022_Moranz_Asclepias/Moranz-AsclepiasCollab/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick.lyon/Documents/Publications/2022_Moranz_Asclepias/Moranz-AsclepiasCollab/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBEAA242-41D8-A44A-A043-C89B007F1E18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6705A23F-5B68-904E-A383-B27394993B85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="600" windowWidth="27360" windowHeight="16760" activeTab="3" xr2:uid="{11370D87-3625-934B-A86E-98D4B25C608F}"/>
+    <workbookView xWindow="380" yWindow="600" windowWidth="27360" windowHeight="16760" activeTab="1" xr2:uid="{11370D87-3625-934B-A86E-98D4B25C608F}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Dictionary" sheetId="9" r:id="rId1"/>
@@ -1702,11 +1702,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B567C001-4211-2141-A4C0-E003D00B102E}">
-  <dimension ref="A1:B88"/>
+  <dimension ref="A1:B106"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B106" sqref="B106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2416,6 +2416,150 @@
       </c>
       <c r="B88" s="3">
         <v>226</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" s="23">
+        <v>8.15</v>
+      </c>
+      <c r="B89" s="3">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" s="23">
+        <v>8.16</v>
+      </c>
+      <c r="B90" s="3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" s="23">
+        <v>8.17</v>
+      </c>
+      <c r="B91" s="3">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" s="23">
+        <v>8.18</v>
+      </c>
+      <c r="B92" s="3">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="23">
+        <v>8.19</v>
+      </c>
+      <c r="B93" s="3">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" s="23">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="B94" s="3">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" s="23">
+        <v>8.2100000000000009</v>
+      </c>
+      <c r="B95" s="3">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" s="23">
+        <v>8.2200000000000006</v>
+      </c>
+      <c r="B96" s="3">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" s="23">
+        <v>8.23</v>
+      </c>
+      <c r="B97" s="3">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" s="23">
+        <v>8.24</v>
+      </c>
+      <c r="B98" s="3">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" s="23">
+        <v>8.25</v>
+      </c>
+      <c r="B99" s="3">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" s="23">
+        <v>8.26</v>
+      </c>
+      <c r="B100" s="3">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" s="23">
+        <v>8.27</v>
+      </c>
+      <c r="B101" s="3">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" s="23">
+        <v>8.2799999999999994</v>
+      </c>
+      <c r="B102" s="3">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" s="23">
+        <v>8.2899999999999991</v>
+      </c>
+      <c r="B103" s="3">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" s="23">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="B104" s="3">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" s="23">
+        <v>8.31</v>
+      </c>
+      <c r="B105" s="3">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" s="23">
+        <v>9.01</v>
+      </c>
+      <c r="B106" s="3">
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -7571,7 +7715,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75508629-25B2-6040-B681-F3ECCEADD070}">
   <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
     </sheetView>

</xml_diff>